<commit_message>
vault backup: 2023-03-08 14:33:59
</commit_message>
<xml_diff>
--- a/Algorithms/Decision_Tree/Entr_Calc.xlsx
+++ b/Algorithms/Decision_Tree/Entr_Calc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22325"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\A000 Next Step\B10 - Machine Learning &amp; AI\A00-ML\0  Oracle ML\Day3\Decision_Tree\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TASUMANT\personal\DSandML\Algorithms\Decision_Tree\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B5770E3-9D11-4454-895D-DD258DA4F7F8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{536BA1FD-6135-4DA9-BFA8-068E64F98AEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5959A98F-6088-4018-90FC-CD330817867A}"/>
+    <workbookView xWindow="-11400" yWindow="10690" windowWidth="19420" windowHeight="10300" xr2:uid="{5959A98F-6088-4018-90FC-CD330817867A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -161,7 +161,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -183,6 +183,7 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -500,12 +501,12 @@
   <dimension ref="A1:I3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
@@ -517,7 +518,7 @@
       <c r="F1" s="10"/>
       <c r="G1" s="10"/>
     </row>
-    <row r="2" spans="1:9" ht="15.6" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -540,35 +541,35 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="4">
-        <v>0</v>
-      </c>
-      <c r="B3" s="4" t="e">
+    <row r="3" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="11">
+        <v>0.8</v>
+      </c>
+      <c r="B3" s="4">
         <f>LOG(A3,2)</f>
-        <v>#NUM!</v>
-      </c>
-      <c r="C3" s="4" t="e">
+        <v>-0.32192809488736229</v>
+      </c>
+      <c r="C3" s="4">
         <f t="shared" ref="C3" si="0">A3*B3</f>
-        <v>#NUM!</v>
+        <v>-0.25754247590988982</v>
       </c>
       <c r="D3" s="5"/>
       <c r="E3" s="6">
         <f t="shared" ref="E3" si="1">1-A3</f>
-        <v>1</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="F3" s="6">
         <f t="shared" ref="F3" si="2">LOG(E3,2)</f>
-        <v>0</v>
+        <v>-2.3219280948873626</v>
       </c>
       <c r="G3" s="6">
         <f t="shared" ref="G3" si="3">E3*F3</f>
-        <v>0</v>
+        <v>-0.46438561897747244</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="8" t="e">
+      <c r="I3" s="8">
         <f t="shared" ref="I3" si="4">-C3-G3</f>
-        <v>#NUM!</v>
+        <v>0.72192809488736231</v>
       </c>
     </row>
   </sheetData>

</xml_diff>